<commit_message>
FIX: added export for a few classes added import for persons added basic login
</commit_message>
<xml_diff>
--- a/persons.xlsx
+++ b/persons.xlsx
@@ -6,21 +6,30 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="person" r:id="rId3" sheetId="1"/>
+    <sheet name="data" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Surname</t>
-  </si>
-  <si>
-    <t>Personcode</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+  <si>
+    <t>idp</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>surname</t>
+  </si>
+  <si>
+    <t>personcode</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>John</t>
@@ -32,12 +41,24 @@
     <t>123456-89012</t>
   </si>
   <si>
+    <t>lv.venta.models.users.User@1722d96b</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>Jane</t>
   </si>
   <si>
     <t>Smith</t>
   </si>
   <si>
+    <t>lv.venta.models.users.User@211496df</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Karina</t>
   </si>
   <si>
@@ -47,6 +68,12 @@
     <t>121212-12121</t>
   </si>
   <si>
+    <t>lv.venta.models.users.User@783d5f65</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Karlis</t>
   </si>
   <si>
@@ -56,6 +83,12 @@
     <t>121212-12123</t>
   </si>
   <si>
+    <t>lv.venta.models.users.User@55d764b9</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>Janis</t>
   </si>
   <si>
@@ -65,6 +98,12 @@
     <t>211221-34567</t>
   </si>
   <si>
+    <t>lv.venta.models.users.User@30fcecfb</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>Baiba</t>
   </si>
   <si>
@@ -74,6 +113,12 @@
     <t>121256-98765</t>
   </si>
   <si>
+    <t>lv.venta.models.users.User@158e727</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Andris</t>
   </si>
   <si>
@@ -81,6 +126,9 @@
   </si>
   <si>
     <t>131256-98765</t>
+  </si>
+  <si>
+    <t>lv.venta.models.users.User@6147b2ee</t>
   </si>
 </sst>
 </file>
@@ -125,7 +173,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -141,82 +189,130 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>